<commit_message>
CF1: full scan, main rules (interval, sept, tritone, stagnation, note repeat). Centralized chunk logs. Fixes
</commit_message>
<xml_diff>
--- a/MGen/isaac-default-random.xlsx
+++ b/MGen/isaac-default-random.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="84" windowWidth="22980" windowHeight="8484" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="84" windowWidth="22980" windowHeight="8484" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Диаграмма1" sheetId="2" r:id="rId1"/>
@@ -604,37 +604,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9099</c:v>
+                  <c:v>9134</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9086</c:v>
+                  <c:v>9081</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9102</c:v>
+                  <c:v>9115</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9080</c:v>
+                  <c:v>9017</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>9246</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9164</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9126</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8964</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9197</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>9051</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>9221</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8933</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9122</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9032</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9286</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>8988</c:v>
+                  <c:v>8901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -654,37 +654,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9285</c:v>
+                  <c:v>9197</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9070</c:v>
+                  <c:v>9057</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8917</c:v>
+                  <c:v>9110</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9071</c:v>
+                  <c:v>9236</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9138</c:v>
+                  <c:v>8899</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9001</c:v>
+                  <c:v>9124</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8989</c:v>
+                  <c:v>9069</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9114</c:v>
+                  <c:v>9094</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9166</c:v>
+                  <c:v>8994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9176</c:v>
+                  <c:v>9160</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9073</c:v>
+                  <c:v>9058</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -704,37 +704,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9187</c:v>
+                  <c:v>9098</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9247</c:v>
+                  <c:v>9144</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9230</c:v>
+                  <c:v>9033</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9079</c:v>
+                  <c:v>9063</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8969</c:v>
+                  <c:v>9099</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9022</c:v>
+                  <c:v>9229</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9145</c:v>
+                  <c:v>9170</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9114</c:v>
+                  <c:v>8941</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9016</c:v>
+                  <c:v>9005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8988</c:v>
+                  <c:v>9090</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9003</c:v>
+                  <c:v>9127</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -754,37 +754,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9150</c:v>
+                  <c:v>9198</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8999</c:v>
+                  <c:v>9148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9022</c:v>
+                  <c:v>8992</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9115</c:v>
+                  <c:v>9089</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9267</c:v>
+                  <c:v>8932</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9166</c:v>
+                  <c:v>8909</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8897</c:v>
+                  <c:v>9149</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9076</c:v>
+                  <c:v>8975</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9047</c:v>
+                  <c:v>9312</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9210</c:v>
+                  <c:v>9186</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9051</c:v>
+                  <c:v>9106</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -804,37 +804,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8983</c:v>
+                  <c:v>9114</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9008</c:v>
+                  <c:v>9063</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9092</c:v>
+                  <c:v>9133</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9172</c:v>
+                  <c:v>8960</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9038</c:v>
+                  <c:v>9018</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9047</c:v>
+                  <c:v>9076</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9136</c:v>
+                  <c:v>9195</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9309</c:v>
+                  <c:v>9052</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9096</c:v>
+                  <c:v>9119</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9077</c:v>
+                  <c:v>9186</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9042</c:v>
+                  <c:v>9082</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -854,37 +854,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9136</c:v>
+                  <c:v>9160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9088</c:v>
+                  <c:v>8974</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9182</c:v>
+                  <c:v>9105</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8998</c:v>
+                  <c:v>9065</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9024</c:v>
+                  <c:v>8995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8991</c:v>
+                  <c:v>9077</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9030</c:v>
+                  <c:v>9145</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9101</c:v>
+                  <c:v>9175</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9183</c:v>
+                  <c:v>9080</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9066</c:v>
+                  <c:v>8990</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9201</c:v>
+                  <c:v>9230</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -904,37 +904,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9233</c:v>
+                  <c:v>9085</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9105</c:v>
+                  <c:v>9119</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8821</c:v>
+                  <c:v>9038</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9131</c:v>
+                  <c:v>9112</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9022</c:v>
+                  <c:v>9018</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9280</c:v>
+                  <c:v>9026</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>9065</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>9134</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>9046</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>9046</c:v>
+                  <c:v>9250</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9130</c:v>
+                  <c:v>9030</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9052</c:v>
+                  <c:v>9119</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -954,37 +954,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9115</c:v>
+                  <c:v>9153</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8943</c:v>
+                  <c:v>9179</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9233</c:v>
+                  <c:v>9100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9064</c:v>
+                  <c:v>9066</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9034</c:v>
+                  <c:v>9101</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8988</c:v>
+                  <c:v>9020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9022</c:v>
+                  <c:v>9042</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9237</c:v>
+                  <c:v>9117</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9067</c:v>
+                  <c:v>9147</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9306</c:v>
+                  <c:v>8985</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8991</c:v>
+                  <c:v>9087</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1004,37 +1004,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8991</c:v>
+                  <c:v>9173</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9133</c:v>
+                  <c:v>9054</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8976</c:v>
+                  <c:v>9172</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8973</c:v>
+                  <c:v>9087</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9159</c:v>
+                  <c:v>9108</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8993</c:v>
+                  <c:v>9070</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9196</c:v>
+                  <c:v>9047</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9064</c:v>
+                  <c:v>9086</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9184</c:v>
+                  <c:v>9003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9142</c:v>
+                  <c:v>9110</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9189</c:v>
+                  <c:v>9084</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1054,37 +1054,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9117</c:v>
+                  <c:v>9149</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9047</c:v>
+                  <c:v>9360</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9011</c:v>
+                  <c:v>9147</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9396</c:v>
+                  <c:v>9097</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9069</c:v>
+                  <c:v>9046</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9087</c:v>
+                  <c:v>9032</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9052</c:v>
+                  <c:v>8956</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9082</c:v>
+                  <c:v>9195</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9162</c:v>
+                  <c:v>8980</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8949</c:v>
+                  <c:v>9062</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9028</c:v>
+                  <c:v>8972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1104,37 +1104,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9234</c:v>
+                  <c:v>9229</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8956</c:v>
+                  <c:v>8993</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9002</c:v>
+                  <c:v>9109</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8887</c:v>
+                  <c:v>9184</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9181</c:v>
+                  <c:v>9091</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9118</c:v>
+                  <c:v>9015</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8933</c:v>
+                  <c:v>9240</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9301</c:v>
+                  <c:v>9009</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9072</c:v>
+                  <c:v>9266</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9066</c:v>
+                  <c:v>8973</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9250</c:v>
+                  <c:v>8889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1154,37 +1154,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9098</c:v>
+                  <c:v>9127</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9000</c:v>
+                  <c:v>9084</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9141</c:v>
+                  <c:v>9032</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9086</c:v>
+                  <c:v>9228</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9183</c:v>
+                  <c:v>9037</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9151</c:v>
+                  <c:v>8933</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9127</c:v>
+                  <c:v>9268</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9168</c:v>
+                  <c:v>9108</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8912</c:v>
+                  <c:v>9136</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9115</c:v>
+                  <c:v>9023</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9019</c:v>
+                  <c:v>9020</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1204,37 +1204,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9181</c:v>
+                  <c:v>8992</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9112</c:v>
+                  <c:v>9120</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9159</c:v>
+                  <c:v>9123</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9117</c:v>
+                  <c:v>9164</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9068</c:v>
+                  <c:v>9009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8985</c:v>
+                  <c:v>9261</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9037</c:v>
+                  <c:v>9084</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9055</c:v>
+                  <c:v>9005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9162</c:v>
+                  <c:v>9021</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9129</c:v>
+                  <c:v>9151</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8995</c:v>
+                  <c:v>9070</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1254,37 +1254,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9262</c:v>
+                  <c:v>9237</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9066</c:v>
+                  <c:v>9094</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9114</c:v>
+                  <c:v>9036</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8996</c:v>
+                  <c:v>9071</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8973</c:v>
+                  <c:v>9087</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8947</c:v>
+                  <c:v>9155</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9095</c:v>
+                  <c:v>9163</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9119</c:v>
+                  <c:v>9126</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8976</c:v>
+                  <c:v>8878</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9240</c:v>
+                  <c:v>8966</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9212</c:v>
+                  <c:v>9182</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1304,37 +1304,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9155</c:v>
+                  <c:v>9122</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9043</c:v>
+                  <c:v>9217</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9183</c:v>
+                  <c:v>9038</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9117</c:v>
+                  <c:v>9114</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9039</c:v>
+                  <c:v>9247</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9035</c:v>
+                  <c:v>9065</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9055</c:v>
+                  <c:v>9028</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9062</c:v>
+                  <c:v>9076</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9115</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9079</c:v>
+                  <c:v>8985</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9117</c:v>
+                  <c:v>9103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1354,37 +1354,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8989</c:v>
+                  <c:v>9055</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9157</c:v>
+                  <c:v>9128</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9160</c:v>
+                  <c:v>8907</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8988</c:v>
+                  <c:v>9204</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9250</c:v>
+                  <c:v>8970</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9073</c:v>
+                  <c:v>9110</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9086</c:v>
+                  <c:v>9274</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9047</c:v>
+                  <c:v>9129</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9080</c:v>
+                  <c:v>9078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9054</c:v>
+                  <c:v>9158</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9116</c:v>
+                  <c:v>8981</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1404,37 +1404,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9012</c:v>
+                  <c:v>9114</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9138</c:v>
+                  <c:v>9123</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9034</c:v>
+                  <c:v>9032</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9072</c:v>
+                  <c:v>9118</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9150</c:v>
+                  <c:v>9117</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9048</c:v>
+                  <c:v>9064</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9167</c:v>
+                  <c:v>8930</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9208</c:v>
+                  <c:v>9250</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9040</c:v>
+                  <c:v>9225</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9143</c:v>
+                  <c:v>8949</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8988</c:v>
+                  <c:v>9076</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1454,37 +1454,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9003</c:v>
+                  <c:v>9143</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8958</c:v>
+                  <c:v>9135</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9061</c:v>
+                  <c:v>9025</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9028</c:v>
+                  <c:v>9030</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9138</c:v>
+                  <c:v>8966</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9211</c:v>
+                  <c:v>9101</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9054</c:v>
+                  <c:v>9093</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9329</c:v>
+                  <c:v>8951</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9109</c:v>
+                  <c:v>9267</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9151</c:v>
+                  <c:v>9078</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8958</c:v>
+                  <c:v>9207</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1504,37 +1504,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9067</c:v>
+                  <c:v>9065</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9212</c:v>
+                  <c:v>9082</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9065</c:v>
+                  <c:v>9132</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9119</c:v>
+                  <c:v>9050</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9347</c:v>
+                  <c:v>8990</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9035</c:v>
+                  <c:v>8977</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8949</c:v>
+                  <c:v>9084</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8997</c:v>
+                  <c:v>9213</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9229</c:v>
+                  <c:v>9113</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8948</c:v>
+                  <c:v>9116</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9032</c:v>
+                  <c:v>9173</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1554,37 +1554,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9018</c:v>
+                  <c:v>9028</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9202</c:v>
+                  <c:v>9156</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9073</c:v>
+                  <c:v>9157</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9075</c:v>
+                  <c:v>8973</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9255</c:v>
+                  <c:v>9180</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9220</c:v>
+                  <c:v>8936</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9048</c:v>
+                  <c:v>8995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9224</c:v>
+                  <c:v>9166</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8988</c:v>
+                  <c:v>9203</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8849</c:v>
+                  <c:v>9090</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9048</c:v>
+                  <c:v>9111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1604,37 +1604,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9171</c:v>
+                  <c:v>9043</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9380</c:v>
+                  <c:v>8995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9075</c:v>
+                  <c:v>9220</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9077</c:v>
+                  <c:v>9185</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9111</c:v>
+                  <c:v>8962</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8982</c:v>
+                  <c:v>9201</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9047</c:v>
+                  <c:v>9172</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9051</c:v>
+                  <c:v>8979</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8984</c:v>
+                  <c:v>9038</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9044</c:v>
+                  <c:v>9179</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9078</c:v>
+                  <c:v>9023</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1654,37 +1654,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9074</c:v>
+                  <c:v>8938</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9094</c:v>
+                  <c:v>9089</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9208</c:v>
+                  <c:v>9051</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8908</c:v>
+                  <c:v>9210</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9079</c:v>
+                  <c:v>9134</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9044</c:v>
+                  <c:v>8984</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9021</c:v>
+                  <c:v>9176</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9193</c:v>
+                  <c:v>9008</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9143</c:v>
+                  <c:v>9160</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9070</c:v>
+                  <c:v>9056</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9166</c:v>
+                  <c:v>9190</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1704,37 +1704,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9068</c:v>
+                  <c:v>9043</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9014</c:v>
+                  <c:v>9204</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9105</c:v>
+                  <c:v>8975</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9002</c:v>
+                  <c:v>9175</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9136</c:v>
+                  <c:v>9029</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8957</c:v>
+                  <c:v>9094</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9136</c:v>
+                  <c:v>9065</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9015</c:v>
+                  <c:v>9063</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9144</c:v>
+                  <c:v>9083</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9292</c:v>
+                  <c:v>9220</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9131</c:v>
+                  <c:v>9047</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1754,37 +1754,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9004</c:v>
+                  <c:v>9192</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9078</c:v>
+                  <c:v>9052</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8999</c:v>
+                  <c:v>9103</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9150</c:v>
+                  <c:v>9063</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9085</c:v>
+                  <c:v>9133</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9058</c:v>
+                  <c:v>9021</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9080</c:v>
+                  <c:v>9146</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9083</c:v>
+                  <c:v>9053</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9241</c:v>
+                  <c:v>9048</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9160</c:v>
+                  <c:v>9169</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9062</c:v>
+                  <c:v>9018</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1804,37 +1804,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9137</c:v>
+                  <c:v>9256</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9119</c:v>
+                  <c:v>9043</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9085</c:v>
+                  <c:v>9222</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9081</c:v>
+                  <c:v>9152</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9121</c:v>
+                  <c:v>9073</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8987</c:v>
+                  <c:v>8912</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9220</c:v>
+                  <c:v>9007</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9121</c:v>
+                  <c:v>9065</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9121</c:v>
+                  <c:v>9110</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8979</c:v>
+                  <c:v>8914</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9029</c:v>
+                  <c:v>9246</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1854,37 +1854,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9040</c:v>
+                  <c:v>9018</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9101</c:v>
+                  <c:v>9020</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>9141</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9166</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8941</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8937</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9126</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8980</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9308</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>9231</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9107</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9061</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9074</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9061</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9175</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9068</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9069</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1904,37 +1904,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9048</c:v>
+                  <c:v>8979</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9112</c:v>
+                  <c:v>8908</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9019</c:v>
+                  <c:v>9146</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9091</c:v>
+                  <c:v>9060</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9039</c:v>
+                  <c:v>9101</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9083</c:v>
+                  <c:v>9239</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8961</c:v>
+                  <c:v>9170</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9342</c:v>
+                  <c:v>8954</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9225</c:v>
+                  <c:v>9209</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9109</c:v>
+                  <c:v>9162</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8971</c:v>
+                  <c:v>9070</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1954,37 +1954,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9185</c:v>
+                  <c:v>9269</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9053</c:v>
+                  <c:v>9037</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9118</c:v>
+                  <c:v>9020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9038</c:v>
+                  <c:v>9014</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9126</c:v>
+                  <c:v>9178</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9117</c:v>
+                  <c:v>8954</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8986</c:v>
+                  <c:v>9200</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8957</c:v>
+                  <c:v>9112</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9065</c:v>
+                  <c:v>9138</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9113</c:v>
+                  <c:v>8916</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9242</c:v>
+                  <c:v>9160</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2004,37 +2004,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9165</c:v>
+                  <c:v>9122</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9111</c:v>
+                  <c:v>9090</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9193</c:v>
+                  <c:v>9128</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9136</c:v>
+                  <c:v>8949</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9011</c:v>
+                  <c:v>9060</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9040</c:v>
+                  <c:v>9218</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9015</c:v>
+                  <c:v>9134</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8893</c:v>
+                  <c:v>9229</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9198</c:v>
+                  <c:v>8901</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9142</c:v>
+                  <c:v>9073</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9096</c:v>
+                  <c:v>9093</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2054,37 +2054,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9078</c:v>
+                  <c:v>9030</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9210</c:v>
+                  <c:v>9075</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8974</c:v>
+                  <c:v>9191</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9217</c:v>
+                  <c:v>9211</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9127</c:v>
+                  <c:v>9112</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9113</c:v>
+                  <c:v>9005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9065</c:v>
+                  <c:v>8958</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9056</c:v>
+                  <c:v>9172</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9007</c:v>
+                  <c:v>9142</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8914</c:v>
+                  <c:v>8979</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9239</c:v>
+                  <c:v>9121</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2184,94 +2184,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>9099</c:v>
+                  <c:v>9134</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9285</c:v>
+                  <c:v>9197</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9187</c:v>
+                  <c:v>9098</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9150</c:v>
+                  <c:v>9198</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8983</c:v>
+                  <c:v>9114</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9136</c:v>
+                  <c:v>9160</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9233</c:v>
+                  <c:v>9085</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9115</c:v>
+                  <c:v>9153</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8991</c:v>
+                  <c:v>9173</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9117</c:v>
+                  <c:v>9149</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9234</c:v>
+                  <c:v>9229</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9098</c:v>
+                  <c:v>9127</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9181</c:v>
+                  <c:v>8992</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9262</c:v>
+                  <c:v>9237</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9155</c:v>
+                  <c:v>9122</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8989</c:v>
+                  <c:v>9055</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9012</c:v>
+                  <c:v>9114</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9003</c:v>
+                  <c:v>9143</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9067</c:v>
+                  <c:v>9065</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>9028</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9043</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8938</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9043</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9192</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9256</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>9018</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>9171</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>9074</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>9068</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>9004</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>9137</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>9040</c:v>
-                </c:pt>
                 <c:pt idx="26">
-                  <c:v>9048</c:v>
+                  <c:v>8979</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9185</c:v>
+                  <c:v>9269</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9165</c:v>
+                  <c:v>9122</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9078</c:v>
+                  <c:v>9030</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2291,94 +2291,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>9086</c:v>
+                  <c:v>9081</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9070</c:v>
+                  <c:v>9057</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9247</c:v>
+                  <c:v>9144</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8999</c:v>
+                  <c:v>9148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9008</c:v>
+                  <c:v>9063</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9088</c:v>
+                  <c:v>8974</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9105</c:v>
+                  <c:v>9119</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8943</c:v>
+                  <c:v>9179</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9133</c:v>
+                  <c:v>9054</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9047</c:v>
+                  <c:v>9360</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8956</c:v>
+                  <c:v>8993</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9000</c:v>
+                  <c:v>9084</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9112</c:v>
+                  <c:v>9120</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9066</c:v>
+                  <c:v>9094</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>9217</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9128</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9123</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9135</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9082</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9156</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8995</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9089</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9204</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9052</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>9043</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>9157</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>9138</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8958</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9212</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9202</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9380</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>9094</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>9014</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>9078</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>9119</c:v>
-                </c:pt>
                 <c:pt idx="25">
-                  <c:v>9101</c:v>
+                  <c:v>9020</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>9112</c:v>
+                  <c:v>8908</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9053</c:v>
+                  <c:v>9037</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9111</c:v>
+                  <c:v>9090</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9210</c:v>
+                  <c:v>9075</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2398,94 +2398,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>9102</c:v>
+                  <c:v>9115</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8917</c:v>
+                  <c:v>9110</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9230</c:v>
+                  <c:v>9033</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9022</c:v>
+                  <c:v>8992</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9092</c:v>
+                  <c:v>9133</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9182</c:v>
+                  <c:v>9105</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8821</c:v>
+                  <c:v>9038</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9233</c:v>
+                  <c:v>9100</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8976</c:v>
+                  <c:v>9172</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9011</c:v>
+                  <c:v>9147</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9002</c:v>
+                  <c:v>9109</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>9032</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9123</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9036</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9038</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8907</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9032</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9025</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9132</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9157</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9220</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9051</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8975</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9103</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9222</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>9141</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>9159</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>9114</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9183</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>9160</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>9034</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>9061</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9065</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9073</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9075</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>9208</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>9105</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>8999</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>9085</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>9231</c:v>
-                </c:pt>
                 <c:pt idx="26">
-                  <c:v>9019</c:v>
+                  <c:v>9146</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9118</c:v>
+                  <c:v>9020</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9193</c:v>
+                  <c:v>9128</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>8974</c:v>
+                  <c:v>9191</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2505,94 +2505,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>9080</c:v>
+                  <c:v>9017</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>9236</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9063</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9089</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8960</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9065</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9112</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9066</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9087</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9097</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9184</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9228</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9164</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>9071</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>9079</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9115</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9172</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9131</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9064</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="14">
+                  <c:v>9114</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9204</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9118</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9030</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9050</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>8973</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>9396</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8887</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9086</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9117</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8996</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9117</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>8988</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>9072</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>9028</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9119</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9075</c:v>
-                </c:pt>
                 <c:pt idx="20">
-                  <c:v>9077</c:v>
+                  <c:v>9185</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8908</c:v>
+                  <c:v>9210</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9002</c:v>
+                  <c:v>9175</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9150</c:v>
+                  <c:v>9063</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9081</c:v>
+                  <c:v>9152</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9107</c:v>
+                  <c:v>9125</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>9091</c:v>
+                  <c:v>9060</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9038</c:v>
+                  <c:v>9014</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9136</c:v>
+                  <c:v>8949</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9217</c:v>
+                  <c:v>9211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2612,94 +2612,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>9051</c:v>
+                  <c:v>9246</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9138</c:v>
+                  <c:v>8899</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8969</c:v>
+                  <c:v>9099</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9267</c:v>
+                  <c:v>8932</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9038</c:v>
+                  <c:v>9018</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9024</c:v>
+                  <c:v>8995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9022</c:v>
+                  <c:v>9018</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9034</c:v>
+                  <c:v>9101</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9159</c:v>
+                  <c:v>9108</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9069</c:v>
+                  <c:v>9046</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9181</c:v>
+                  <c:v>9091</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9183</c:v>
+                  <c:v>9037</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9068</c:v>
+                  <c:v>9009</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8973</c:v>
+                  <c:v>9087</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9039</c:v>
+                  <c:v>9247</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9250</c:v>
+                  <c:v>8970</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9150</c:v>
+                  <c:v>9117</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9138</c:v>
+                  <c:v>8966</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9347</c:v>
+                  <c:v>8990</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9255</c:v>
+                  <c:v>9180</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9111</c:v>
+                  <c:v>8962</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9079</c:v>
+                  <c:v>9134</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9136</c:v>
+                  <c:v>9029</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9085</c:v>
+                  <c:v>9133</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9121</c:v>
+                  <c:v>9073</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9061</c:v>
+                  <c:v>9166</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>9039</c:v>
+                  <c:v>9101</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9126</c:v>
+                  <c:v>9178</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9011</c:v>
+                  <c:v>9060</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9127</c:v>
+                  <c:v>9112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2719,94 +2719,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>9221</c:v>
+                  <c:v>9164</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9001</c:v>
+                  <c:v>9124</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9022</c:v>
+                  <c:v>9229</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9166</c:v>
+                  <c:v>8909</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9047</c:v>
+                  <c:v>9076</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8991</c:v>
+                  <c:v>9077</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9280</c:v>
+                  <c:v>9026</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8988</c:v>
+                  <c:v>9020</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8993</c:v>
+                  <c:v>9070</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9087</c:v>
+                  <c:v>9032</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9118</c:v>
+                  <c:v>9015</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9151</c:v>
+                  <c:v>8933</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8985</c:v>
+                  <c:v>9261</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8947</c:v>
+                  <c:v>9155</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9035</c:v>
+                  <c:v>9065</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9073</c:v>
+                  <c:v>9110</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9048</c:v>
+                  <c:v>9064</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9211</c:v>
+                  <c:v>9101</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9035</c:v>
+                  <c:v>8977</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9220</c:v>
+                  <c:v>8936</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8982</c:v>
+                  <c:v>9201</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9044</c:v>
+                  <c:v>8984</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8957</c:v>
+                  <c:v>9094</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9058</c:v>
+                  <c:v>9021</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8987</c:v>
+                  <c:v>8912</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9074</c:v>
+                  <c:v>8941</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>9083</c:v>
+                  <c:v>9239</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9117</c:v>
+                  <c:v>8954</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9040</c:v>
+                  <c:v>9218</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9113</c:v>
+                  <c:v>9005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2826,94 +2826,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>8933</c:v>
+                  <c:v>9126</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8989</c:v>
+                  <c:v>9069</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>9170</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9149</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9195</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>9145</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>8897</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9136</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9030</c:v>
-                </c:pt>
                 <c:pt idx="6">
+                  <c:v>9065</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9042</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9047</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8956</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9240</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9268</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9084</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9163</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9028</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9274</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8930</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9093</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9084</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8995</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9172</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9176</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9065</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9146</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9007</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8937</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9170</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9200</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>9134</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>9022</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9196</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9052</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8933</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9127</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9037</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>9095</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9055</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>9086</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>9167</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>9054</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>8949</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9048</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9047</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>9021</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>9136</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>9080</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>9220</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>9061</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>8961</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>8986</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>9015</c:v>
-                </c:pt>
                 <c:pt idx="29">
-                  <c:v>9065</c:v>
+                  <c:v>8958</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2933,94 +2933,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>9122</c:v>
+                  <c:v>8964</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9114</c:v>
+                  <c:v>9094</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9114</c:v>
+                  <c:v>8941</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>8975</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9052</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9175</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9134</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9117</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9086</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9195</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9009</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9108</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9005</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9126</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>9076</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>9309</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9101</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9046</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9237</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9064</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9082</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9301</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9168</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9055</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>9119</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9062</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>9047</c:v>
+                  <c:v>9129</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9208</c:v>
+                  <c:v>9250</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9329</c:v>
+                  <c:v>8951</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8997</c:v>
+                  <c:v>9213</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9224</c:v>
+                  <c:v>9166</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9051</c:v>
+                  <c:v>8979</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9193</c:v>
+                  <c:v>9008</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9015</c:v>
+                  <c:v>9063</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9083</c:v>
+                  <c:v>9053</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9121</c:v>
+                  <c:v>9065</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9175</c:v>
+                  <c:v>9126</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>9342</c:v>
+                  <c:v>8954</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8957</c:v>
+                  <c:v>9112</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>8893</c:v>
+                  <c:v>9229</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9056</c:v>
+                  <c:v>9172</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3040,94 +3040,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>9032</c:v>
+                  <c:v>9197</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9166</c:v>
+                  <c:v>8994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9016</c:v>
+                  <c:v>9005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9047</c:v>
+                  <c:v>9312</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9096</c:v>
+                  <c:v>9119</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9183</c:v>
+                  <c:v>9080</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9046</c:v>
+                  <c:v>9250</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9067</c:v>
+                  <c:v>9147</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9184</c:v>
+                  <c:v>9003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9162</c:v>
+                  <c:v>8980</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9072</c:v>
+                  <c:v>9266</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8912</c:v>
+                  <c:v>9136</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9162</c:v>
+                  <c:v>9021</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8976</c:v>
+                  <c:v>8878</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9115</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9080</c:v>
+                  <c:v>9078</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9040</c:v>
+                  <c:v>9225</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9109</c:v>
+                  <c:v>9267</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9229</c:v>
+                  <c:v>9113</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8988</c:v>
+                  <c:v>9203</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8984</c:v>
+                  <c:v>9038</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9143</c:v>
+                  <c:v>9160</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9144</c:v>
+                  <c:v>9083</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9241</c:v>
+                  <c:v>9048</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9121</c:v>
+                  <c:v>9110</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9068</c:v>
+                  <c:v>8980</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>9225</c:v>
+                  <c:v>9209</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9065</c:v>
+                  <c:v>9138</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9198</c:v>
+                  <c:v>8901</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9007</c:v>
+                  <c:v>9142</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3147,94 +3147,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>9286</c:v>
+                  <c:v>9051</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9176</c:v>
+                  <c:v>9160</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8988</c:v>
+                  <c:v>9090</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9210</c:v>
+                  <c:v>9186</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9077</c:v>
+                  <c:v>9186</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9066</c:v>
+                  <c:v>8990</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9130</c:v>
+                  <c:v>9030</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9306</c:v>
+                  <c:v>8985</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9142</c:v>
+                  <c:v>9110</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>9062</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8973</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9023</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9151</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8966</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8985</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9158</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>8949</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>9066</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9115</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9129</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>9240</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9079</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>9054</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>9143</c:v>
-                </c:pt>
                 <c:pt idx="17">
-                  <c:v>9151</c:v>
+                  <c:v>9078</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8948</c:v>
+                  <c:v>9116</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8849</c:v>
+                  <c:v>9090</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9044</c:v>
+                  <c:v>9179</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9070</c:v>
+                  <c:v>9056</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9292</c:v>
+                  <c:v>9220</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9160</c:v>
+                  <c:v>9169</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>8914</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9308</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9162</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8916</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9073</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>8979</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>9069</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>9109</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>9113</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>9142</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>8914</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3254,94 +3254,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>8988</c:v>
+                  <c:v>8901</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9073</c:v>
+                  <c:v>9058</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9003</c:v>
+                  <c:v>9127</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9051</c:v>
+                  <c:v>9106</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9042</c:v>
+                  <c:v>9082</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9201</c:v>
+                  <c:v>9230</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9052</c:v>
+                  <c:v>9119</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8991</c:v>
+                  <c:v>9087</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9189</c:v>
+                  <c:v>9084</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9028</c:v>
+                  <c:v>8972</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9250</c:v>
+                  <c:v>8889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9019</c:v>
+                  <c:v>9020</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8995</c:v>
+                  <c:v>9070</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9212</c:v>
+                  <c:v>9182</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9117</c:v>
+                  <c:v>9103</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9116</c:v>
+                  <c:v>8981</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8988</c:v>
+                  <c:v>9076</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8958</c:v>
+                  <c:v>9207</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9032</c:v>
+                  <c:v>9173</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9048</c:v>
+                  <c:v>9111</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9078</c:v>
+                  <c:v>9023</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9166</c:v>
+                  <c:v>9190</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9131</c:v>
+                  <c:v>9047</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9062</c:v>
+                  <c:v>9018</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9029</c:v>
+                  <c:v>9246</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9013</c:v>
+                  <c:v>9231</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8971</c:v>
+                  <c:v>9070</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9242</c:v>
+                  <c:v>9160</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9096</c:v>
+                  <c:v>9093</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9239</c:v>
+                  <c:v>9121</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3437,37 +3437,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9109.5</c:v>
+                  <c:v>9115.4333333333325</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9094.7333333333336</c:v>
+                  <c:v>9094.1333333333332</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9086.1666666666661</c:v>
+                  <c:v>9091.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9079.0333333333328</c:v>
+                  <c:v>9102.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9108.3666666666668</c:v>
+                  <c:v>9070.1333333333332</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9069.1333333333332</c:v>
+                  <c:v>9063.7666666666664</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9055.9</c:v>
+                  <c:v>9102.9333333333325</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9122.0333333333328</c:v>
+                  <c:v>9084.2333333333336</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9095.9333333333325</c:v>
+                  <c:v>9102.7666666666664</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9099.8666666666668</c:v>
+                  <c:v>9077.1666666666661</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9079.3333333333339</c:v>
+                  <c:v>9092.5666666666675</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3554,7 +3554,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3931,501 +3931,501 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>9099</v>
+        <v>9134</v>
       </c>
       <c r="B1">
-        <v>9086</v>
+        <v>9081</v>
       </c>
       <c r="C1">
-        <v>9102</v>
+        <v>9115</v>
       </c>
       <c r="D1">
-        <v>9080</v>
+        <v>9017</v>
       </c>
       <c r="E1">
+        <v>9246</v>
+      </c>
+      <c r="F1">
+        <v>9164</v>
+      </c>
+      <c r="G1">
+        <v>9126</v>
+      </c>
+      <c r="H1">
+        <v>8964</v>
+      </c>
+      <c r="I1">
+        <v>9197</v>
+      </c>
+      <c r="J1">
         <v>9051</v>
       </c>
-      <c r="F1">
-        <v>9221</v>
-      </c>
-      <c r="G1">
-        <v>8933</v>
-      </c>
-      <c r="H1">
-        <v>9122</v>
-      </c>
-      <c r="I1">
-        <v>9032</v>
-      </c>
-      <c r="J1">
-        <v>9286</v>
-      </c>
       <c r="K1">
-        <v>8988</v>
+        <v>8901</v>
       </c>
       <c r="L1">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>9285</v>
+        <v>9197</v>
       </c>
       <c r="B2">
-        <v>9070</v>
+        <v>9057</v>
       </c>
       <c r="C2">
-        <v>8917</v>
+        <v>9110</v>
       </c>
       <c r="D2">
-        <v>9071</v>
+        <v>9236</v>
       </c>
       <c r="E2">
-        <v>9138</v>
+        <v>8899</v>
       </c>
       <c r="F2">
-        <v>9001</v>
+        <v>9124</v>
       </c>
       <c r="G2">
-        <v>8989</v>
+        <v>9069</v>
       </c>
       <c r="H2">
-        <v>9114</v>
+        <v>9094</v>
       </c>
       <c r="I2">
-        <v>9166</v>
+        <v>8994</v>
       </c>
       <c r="J2">
-        <v>9176</v>
+        <v>9160</v>
       </c>
       <c r="K2">
-        <v>9073</v>
+        <v>9058</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>9187</v>
+        <v>9098</v>
       </c>
       <c r="B3">
-        <v>9247</v>
+        <v>9144</v>
       </c>
       <c r="C3">
-        <v>9230</v>
+        <v>9033</v>
       </c>
       <c r="D3">
-        <v>9079</v>
+        <v>9063</v>
       </c>
       <c r="E3">
-        <v>8969</v>
+        <v>9099</v>
       </c>
       <c r="F3">
-        <v>9022</v>
+        <v>9229</v>
       </c>
       <c r="G3">
-        <v>9145</v>
+        <v>9170</v>
       </c>
       <c r="H3">
-        <v>9114</v>
+        <v>8941</v>
       </c>
       <c r="I3">
-        <v>9016</v>
+        <v>9005</v>
       </c>
       <c r="J3">
-        <v>8988</v>
+        <v>9090</v>
       </c>
       <c r="K3">
-        <v>9003</v>
+        <v>9127</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>9150</v>
+        <v>9198</v>
       </c>
       <c r="B4">
-        <v>8999</v>
+        <v>9148</v>
       </c>
       <c r="C4">
-        <v>9022</v>
+        <v>8992</v>
       </c>
       <c r="D4">
-        <v>9115</v>
+        <v>9089</v>
       </c>
       <c r="E4">
-        <v>9267</v>
+        <v>8932</v>
       </c>
       <c r="F4">
-        <v>9166</v>
+        <v>8909</v>
       </c>
       <c r="G4">
-        <v>8897</v>
+        <v>9149</v>
       </c>
       <c r="H4">
-        <v>9076</v>
+        <v>8975</v>
       </c>
       <c r="I4">
-        <v>9047</v>
+        <v>9312</v>
       </c>
       <c r="J4">
-        <v>9210</v>
+        <v>9186</v>
       </c>
       <c r="K4">
-        <v>9051</v>
+        <v>9106</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>8983</v>
+        <v>9114</v>
       </c>
       <c r="B5">
-        <v>9008</v>
+        <v>9063</v>
       </c>
       <c r="C5">
-        <v>9092</v>
+        <v>9133</v>
       </c>
       <c r="D5">
-        <v>9172</v>
+        <v>8960</v>
       </c>
       <c r="E5">
-        <v>9038</v>
+        <v>9018</v>
       </c>
       <c r="F5">
-        <v>9047</v>
+        <v>9076</v>
       </c>
       <c r="G5">
-        <v>9136</v>
+        <v>9195</v>
       </c>
       <c r="H5">
-        <v>9309</v>
+        <v>9052</v>
       </c>
       <c r="I5">
-        <v>9096</v>
+        <v>9119</v>
       </c>
       <c r="J5">
-        <v>9077</v>
+        <v>9186</v>
       </c>
       <c r="K5">
-        <v>9042</v>
+        <v>9082</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>9136</v>
+        <v>9160</v>
       </c>
       <c r="B6">
-        <v>9088</v>
+        <v>8974</v>
       </c>
       <c r="C6">
-        <v>9182</v>
+        <v>9105</v>
       </c>
       <c r="D6">
-        <v>8998</v>
+        <v>9065</v>
       </c>
       <c r="E6">
-        <v>9024</v>
+        <v>8995</v>
       </c>
       <c r="F6">
-        <v>8991</v>
+        <v>9077</v>
       </c>
       <c r="G6">
-        <v>9030</v>
+        <v>9145</v>
       </c>
       <c r="H6">
-        <v>9101</v>
+        <v>9175</v>
       </c>
       <c r="I6">
-        <v>9183</v>
+        <v>9080</v>
       </c>
       <c r="J6">
-        <v>9066</v>
+        <v>8990</v>
       </c>
       <c r="K6">
-        <v>9201</v>
+        <v>9230</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>9233</v>
+        <v>9085</v>
       </c>
       <c r="B7">
-        <v>9105</v>
+        <v>9119</v>
       </c>
       <c r="C7">
-        <v>8821</v>
+        <v>9038</v>
       </c>
       <c r="D7">
-        <v>9131</v>
+        <v>9112</v>
       </c>
       <c r="E7">
-        <v>9022</v>
+        <v>9018</v>
       </c>
       <c r="F7">
-        <v>9280</v>
+        <v>9026</v>
       </c>
       <c r="G7">
+        <v>9065</v>
+      </c>
+      <c r="H7">
         <v>9134</v>
       </c>
-      <c r="H7">
-        <v>9046</v>
-      </c>
       <c r="I7">
-        <v>9046</v>
+        <v>9250</v>
       </c>
       <c r="J7">
-        <v>9130</v>
+        <v>9030</v>
       </c>
       <c r="K7">
-        <v>9052</v>
+        <v>9119</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>9115</v>
+        <v>9153</v>
       </c>
       <c r="B8">
-        <v>8943</v>
+        <v>9179</v>
       </c>
       <c r="C8">
-        <v>9233</v>
+        <v>9100</v>
       </c>
       <c r="D8">
-        <v>9064</v>
+        <v>9066</v>
       </c>
       <c r="E8">
-        <v>9034</v>
+        <v>9101</v>
       </c>
       <c r="F8">
-        <v>8988</v>
+        <v>9020</v>
       </c>
       <c r="G8">
-        <v>9022</v>
+        <v>9042</v>
       </c>
       <c r="H8">
-        <v>9237</v>
+        <v>9117</v>
       </c>
       <c r="I8">
-        <v>9067</v>
+        <v>9147</v>
       </c>
       <c r="J8">
-        <v>9306</v>
+        <v>8985</v>
       </c>
       <c r="K8">
-        <v>8991</v>
+        <v>9087</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8991</v>
+        <v>9173</v>
       </c>
       <c r="B9">
-        <v>9133</v>
+        <v>9054</v>
       </c>
       <c r="C9">
-        <v>8976</v>
+        <v>9172</v>
       </c>
       <c r="D9">
-        <v>8973</v>
+        <v>9087</v>
       </c>
       <c r="E9">
-        <v>9159</v>
+        <v>9108</v>
       </c>
       <c r="F9">
-        <v>8993</v>
+        <v>9070</v>
       </c>
       <c r="G9">
-        <v>9196</v>
+        <v>9047</v>
       </c>
       <c r="H9">
-        <v>9064</v>
+        <v>9086</v>
       </c>
       <c r="I9">
-        <v>9184</v>
+        <v>9003</v>
       </c>
       <c r="J9">
-        <v>9142</v>
+        <v>9110</v>
       </c>
       <c r="K9">
-        <v>9189</v>
+        <v>9084</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>9117</v>
+        <v>9149</v>
       </c>
       <c r="B10">
-        <v>9047</v>
+        <v>9360</v>
       </c>
       <c r="C10">
-        <v>9011</v>
+        <v>9147</v>
       </c>
       <c r="D10">
-        <v>9396</v>
+        <v>9097</v>
       </c>
       <c r="E10">
-        <v>9069</v>
+        <v>9046</v>
       </c>
       <c r="F10">
-        <v>9087</v>
+        <v>9032</v>
       </c>
       <c r="G10">
-        <v>9052</v>
+        <v>8956</v>
       </c>
       <c r="H10">
-        <v>9082</v>
+        <v>9195</v>
       </c>
       <c r="I10">
-        <v>9162</v>
+        <v>8980</v>
       </c>
       <c r="J10">
-        <v>8949</v>
+        <v>9062</v>
       </c>
       <c r="K10">
-        <v>9028</v>
+        <v>8972</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>9234</v>
+        <v>9229</v>
       </c>
       <c r="B11">
-        <v>8956</v>
+        <v>8993</v>
       </c>
       <c r="C11">
-        <v>9002</v>
+        <v>9109</v>
       </c>
       <c r="D11">
-        <v>8887</v>
+        <v>9184</v>
       </c>
       <c r="E11">
-        <v>9181</v>
+        <v>9091</v>
       </c>
       <c r="F11">
-        <v>9118</v>
+        <v>9015</v>
       </c>
       <c r="G11">
-        <v>8933</v>
+        <v>9240</v>
       </c>
       <c r="H11">
-        <v>9301</v>
+        <v>9009</v>
       </c>
       <c r="I11">
-        <v>9072</v>
+        <v>9266</v>
       </c>
       <c r="J11">
-        <v>9066</v>
+        <v>8973</v>
       </c>
       <c r="K11">
-        <v>9250</v>
+        <v>8889</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>9098</v>
+        <v>9127</v>
       </c>
       <c r="B12">
-        <v>9000</v>
+        <v>9084</v>
       </c>
       <c r="C12">
-        <v>9141</v>
+        <v>9032</v>
       </c>
       <c r="D12">
-        <v>9086</v>
+        <v>9228</v>
       </c>
       <c r="E12">
-        <v>9183</v>
+        <v>9037</v>
       </c>
       <c r="F12">
-        <v>9151</v>
+        <v>8933</v>
       </c>
       <c r="G12">
-        <v>9127</v>
+        <v>9268</v>
       </c>
       <c r="H12">
-        <v>9168</v>
+        <v>9108</v>
       </c>
       <c r="I12">
-        <v>8912</v>
+        <v>9136</v>
       </c>
       <c r="J12">
-        <v>9115</v>
+        <v>9023</v>
       </c>
       <c r="K12">
-        <v>9019</v>
+        <v>9020</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>9181</v>
+        <v>8992</v>
       </c>
       <c r="B13">
-        <v>9112</v>
+        <v>9120</v>
       </c>
       <c r="C13">
-        <v>9159</v>
+        <v>9123</v>
       </c>
       <c r="D13">
-        <v>9117</v>
+        <v>9164</v>
       </c>
       <c r="E13">
-        <v>9068</v>
+        <v>9009</v>
       </c>
       <c r="F13">
-        <v>8985</v>
+        <v>9261</v>
       </c>
       <c r="G13">
-        <v>9037</v>
+        <v>9084</v>
       </c>
       <c r="H13">
-        <v>9055</v>
+        <v>9005</v>
       </c>
       <c r="I13">
-        <v>9162</v>
+        <v>9021</v>
       </c>
       <c r="J13">
-        <v>9129</v>
+        <v>9151</v>
       </c>
       <c r="K13">
-        <v>8995</v>
+        <v>9070</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -4433,455 +4433,455 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>9262</v>
+        <v>9237</v>
       </c>
       <c r="B14">
-        <v>9066</v>
+        <v>9094</v>
       </c>
       <c r="C14">
-        <v>9114</v>
+        <v>9036</v>
       </c>
       <c r="D14">
-        <v>8996</v>
+        <v>9071</v>
       </c>
       <c r="E14">
-        <v>8973</v>
+        <v>9087</v>
       </c>
       <c r="F14">
-        <v>8947</v>
+        <v>9155</v>
       </c>
       <c r="G14">
-        <v>9095</v>
+        <v>9163</v>
       </c>
       <c r="H14">
-        <v>9119</v>
+        <v>9126</v>
       </c>
       <c r="I14">
-        <v>8976</v>
+        <v>8878</v>
       </c>
       <c r="J14">
-        <v>9240</v>
+        <v>8966</v>
       </c>
       <c r="K14">
-        <v>9212</v>
+        <v>9182</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>9155</v>
+        <v>9122</v>
       </c>
       <c r="B15">
-        <v>9043</v>
+        <v>9217</v>
       </c>
       <c r="C15">
-        <v>9183</v>
+        <v>9038</v>
       </c>
       <c r="D15">
-        <v>9117</v>
+        <v>9114</v>
       </c>
       <c r="E15">
-        <v>9039</v>
+        <v>9247</v>
       </c>
       <c r="F15">
-        <v>9035</v>
+        <v>9065</v>
       </c>
       <c r="G15">
-        <v>9055</v>
+        <v>9028</v>
       </c>
       <c r="H15">
-        <v>9062</v>
+        <v>9076</v>
       </c>
       <c r="I15">
-        <v>9115</v>
+        <v>9000</v>
       </c>
       <c r="J15">
-        <v>9079</v>
+        <v>8985</v>
       </c>
       <c r="K15">
-        <v>9117</v>
+        <v>9103</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>8989</v>
+        <v>9055</v>
       </c>
       <c r="B16">
-        <v>9157</v>
+        <v>9128</v>
       </c>
       <c r="C16">
-        <v>9160</v>
+        <v>8907</v>
       </c>
       <c r="D16">
-        <v>8988</v>
+        <v>9204</v>
       </c>
       <c r="E16">
-        <v>9250</v>
+        <v>8970</v>
       </c>
       <c r="F16">
-        <v>9073</v>
+        <v>9110</v>
       </c>
       <c r="G16">
-        <v>9086</v>
+        <v>9274</v>
       </c>
       <c r="H16">
-        <v>9047</v>
+        <v>9129</v>
       </c>
       <c r="I16">
-        <v>9080</v>
+        <v>9078</v>
       </c>
       <c r="J16">
-        <v>9054</v>
+        <v>9158</v>
       </c>
       <c r="K16">
-        <v>9116</v>
+        <v>8981</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>9012</v>
+        <v>9114</v>
       </c>
       <c r="B17">
-        <v>9138</v>
+        <v>9123</v>
       </c>
       <c r="C17">
-        <v>9034</v>
+        <v>9032</v>
       </c>
       <c r="D17">
-        <v>9072</v>
+        <v>9118</v>
       </c>
       <c r="E17">
-        <v>9150</v>
+        <v>9117</v>
       </c>
       <c r="F17">
-        <v>9048</v>
+        <v>9064</v>
       </c>
       <c r="G17">
-        <v>9167</v>
+        <v>8930</v>
       </c>
       <c r="H17">
-        <v>9208</v>
+        <v>9250</v>
       </c>
       <c r="I17">
-        <v>9040</v>
+        <v>9225</v>
       </c>
       <c r="J17">
-        <v>9143</v>
+        <v>8949</v>
       </c>
       <c r="K17">
-        <v>8988</v>
+        <v>9076</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>9003</v>
+        <v>9143</v>
       </c>
       <c r="B18">
-        <v>8958</v>
+        <v>9135</v>
       </c>
       <c r="C18">
-        <v>9061</v>
+        <v>9025</v>
       </c>
       <c r="D18">
-        <v>9028</v>
+        <v>9030</v>
       </c>
       <c r="E18">
-        <v>9138</v>
+        <v>8966</v>
       </c>
       <c r="F18">
-        <v>9211</v>
+        <v>9101</v>
       </c>
       <c r="G18">
-        <v>9054</v>
+        <v>9093</v>
       </c>
       <c r="H18">
-        <v>9329</v>
+        <v>8951</v>
       </c>
       <c r="I18">
-        <v>9109</v>
+        <v>9267</v>
       </c>
       <c r="J18">
-        <v>9151</v>
+        <v>9078</v>
       </c>
       <c r="K18">
-        <v>8958</v>
+        <v>9207</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>9067</v>
+        <v>9065</v>
       </c>
       <c r="B19">
-        <v>9212</v>
+        <v>9082</v>
       </c>
       <c r="C19">
-        <v>9065</v>
+        <v>9132</v>
       </c>
       <c r="D19">
-        <v>9119</v>
+        <v>9050</v>
       </c>
       <c r="E19">
-        <v>9347</v>
+        <v>8990</v>
       </c>
       <c r="F19">
-        <v>9035</v>
+        <v>8977</v>
       </c>
       <c r="G19">
-        <v>8949</v>
+        <v>9084</v>
       </c>
       <c r="H19">
-        <v>8997</v>
+        <v>9213</v>
       </c>
       <c r="I19">
-        <v>9229</v>
+        <v>9113</v>
       </c>
       <c r="J19">
-        <v>8948</v>
+        <v>9116</v>
       </c>
       <c r="K19">
-        <v>9032</v>
+        <v>9173</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>9018</v>
+        <v>9028</v>
       </c>
       <c r="B20">
-        <v>9202</v>
+        <v>9156</v>
       </c>
       <c r="C20">
-        <v>9073</v>
+        <v>9157</v>
       </c>
       <c r="D20">
-        <v>9075</v>
+        <v>8973</v>
       </c>
       <c r="E20">
-        <v>9255</v>
+        <v>9180</v>
       </c>
       <c r="F20">
-        <v>9220</v>
+        <v>8936</v>
       </c>
       <c r="G20">
-        <v>9048</v>
+        <v>8995</v>
       </c>
       <c r="H20">
-        <v>9224</v>
+        <v>9166</v>
       </c>
       <c r="I20">
-        <v>8988</v>
+        <v>9203</v>
       </c>
       <c r="J20">
-        <v>8849</v>
+        <v>9090</v>
       </c>
       <c r="K20">
-        <v>9048</v>
+        <v>9111</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>9171</v>
+        <v>9043</v>
       </c>
       <c r="B21">
-        <v>9380</v>
+        <v>8995</v>
       </c>
       <c r="C21">
-        <v>9075</v>
+        <v>9220</v>
       </c>
       <c r="D21">
-        <v>9077</v>
+        <v>9185</v>
       </c>
       <c r="E21">
-        <v>9111</v>
+        <v>8962</v>
       </c>
       <c r="F21">
-        <v>8982</v>
+        <v>9201</v>
       </c>
       <c r="G21">
-        <v>9047</v>
+        <v>9172</v>
       </c>
       <c r="H21">
-        <v>9051</v>
+        <v>8979</v>
       </c>
       <c r="I21">
-        <v>8984</v>
+        <v>9038</v>
       </c>
       <c r="J21">
-        <v>9044</v>
+        <v>9179</v>
       </c>
       <c r="K21">
-        <v>9078</v>
+        <v>9023</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>9074</v>
+        <v>8938</v>
       </c>
       <c r="B22">
-        <v>9094</v>
+        <v>9089</v>
       </c>
       <c r="C22">
-        <v>9208</v>
+        <v>9051</v>
       </c>
       <c r="D22">
-        <v>8908</v>
+        <v>9210</v>
       </c>
       <c r="E22">
-        <v>9079</v>
+        <v>9134</v>
       </c>
       <c r="F22">
-        <v>9044</v>
+        <v>8984</v>
       </c>
       <c r="G22">
-        <v>9021</v>
+        <v>9176</v>
       </c>
       <c r="H22">
-        <v>9193</v>
+        <v>9008</v>
       </c>
       <c r="I22">
-        <v>9143</v>
+        <v>9160</v>
       </c>
       <c r="J22">
-        <v>9070</v>
+        <v>9056</v>
       </c>
       <c r="K22">
-        <v>9166</v>
+        <v>9190</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>9068</v>
+        <v>9043</v>
       </c>
       <c r="B23">
-        <v>9014</v>
+        <v>9204</v>
       </c>
       <c r="C23">
-        <v>9105</v>
+        <v>8975</v>
       </c>
       <c r="D23">
-        <v>9002</v>
+        <v>9175</v>
       </c>
       <c r="E23">
-        <v>9136</v>
+        <v>9029</v>
       </c>
       <c r="F23">
-        <v>8957</v>
+        <v>9094</v>
       </c>
       <c r="G23">
-        <v>9136</v>
+        <v>9065</v>
       </c>
       <c r="H23">
-        <v>9015</v>
+        <v>9063</v>
       </c>
       <c r="I23">
-        <v>9144</v>
+        <v>9083</v>
       </c>
       <c r="J23">
-        <v>9292</v>
+        <v>9220</v>
       </c>
       <c r="K23">
-        <v>9131</v>
+        <v>9047</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>9004</v>
+        <v>9192</v>
       </c>
       <c r="B24">
-        <v>9078</v>
+        <v>9052</v>
       </c>
       <c r="C24">
-        <v>8999</v>
+        <v>9103</v>
       </c>
       <c r="D24">
-        <v>9150</v>
+        <v>9063</v>
       </c>
       <c r="E24">
-        <v>9085</v>
+        <v>9133</v>
       </c>
       <c r="F24">
-        <v>9058</v>
+        <v>9021</v>
       </c>
       <c r="G24">
-        <v>9080</v>
+        <v>9146</v>
       </c>
       <c r="H24">
-        <v>9083</v>
+        <v>9053</v>
       </c>
       <c r="I24">
-        <v>9241</v>
+        <v>9048</v>
       </c>
       <c r="J24">
-        <v>9160</v>
+        <v>9169</v>
       </c>
       <c r="K24">
-        <v>9062</v>
+        <v>9018</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>9137</v>
+        <v>9256</v>
       </c>
       <c r="B25">
-        <v>9119</v>
+        <v>9043</v>
       </c>
       <c r="C25">
-        <v>9085</v>
+        <v>9222</v>
       </c>
       <c r="D25">
-        <v>9081</v>
+        <v>9152</v>
       </c>
       <c r="E25">
-        <v>9121</v>
+        <v>9073</v>
       </c>
       <c r="F25">
-        <v>8987</v>
+        <v>8912</v>
       </c>
       <c r="G25">
-        <v>9220</v>
+        <v>9007</v>
       </c>
       <c r="H25">
-        <v>9121</v>
+        <v>9065</v>
       </c>
       <c r="I25">
-        <v>9121</v>
+        <v>9110</v>
       </c>
       <c r="J25">
-        <v>8979</v>
+        <v>8914</v>
       </c>
       <c r="K25">
-        <v>9029</v>
+        <v>9246</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -4889,238 +4889,238 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>9040</v>
+        <v>9018</v>
       </c>
       <c r="B26">
-        <v>9101</v>
+        <v>9020</v>
       </c>
       <c r="C26">
+        <v>9141</v>
+      </c>
+      <c r="D26">
+        <v>9125</v>
+      </c>
+      <c r="E26">
+        <v>9166</v>
+      </c>
+      <c r="F26">
+        <v>8941</v>
+      </c>
+      <c r="G26">
+        <v>8937</v>
+      </c>
+      <c r="H26">
+        <v>9126</v>
+      </c>
+      <c r="I26">
+        <v>8980</v>
+      </c>
+      <c r="J26">
+        <v>9308</v>
+      </c>
+      <c r="K26">
         <v>9231</v>
       </c>
-      <c r="D26">
-        <v>9107</v>
-      </c>
-      <c r="E26">
-        <v>9061</v>
-      </c>
-      <c r="F26">
-        <v>9074</v>
-      </c>
-      <c r="G26">
-        <v>9061</v>
-      </c>
-      <c r="H26">
-        <v>9175</v>
-      </c>
-      <c r="I26">
-        <v>9068</v>
-      </c>
-      <c r="J26">
-        <v>9069</v>
-      </c>
-      <c r="K26">
-        <v>9013</v>
-      </c>
       <c r="L26">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>9048</v>
+        <v>8979</v>
       </c>
       <c r="B27">
-        <v>9112</v>
+        <v>8908</v>
       </c>
       <c r="C27">
-        <v>9019</v>
+        <v>9146</v>
       </c>
       <c r="D27">
-        <v>9091</v>
+        <v>9060</v>
       </c>
       <c r="E27">
-        <v>9039</v>
+        <v>9101</v>
       </c>
       <c r="F27">
-        <v>9083</v>
+        <v>9239</v>
       </c>
       <c r="G27">
-        <v>8961</v>
+        <v>9170</v>
       </c>
       <c r="H27">
-        <v>9342</v>
+        <v>8954</v>
       </c>
       <c r="I27">
-        <v>9225</v>
+        <v>9209</v>
       </c>
       <c r="J27">
-        <v>9109</v>
+        <v>9162</v>
       </c>
       <c r="K27">
-        <v>8971</v>
+        <v>9070</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>9185</v>
+        <v>9269</v>
       </c>
       <c r="B28">
-        <v>9053</v>
+        <v>9037</v>
       </c>
       <c r="C28">
-        <v>9118</v>
+        <v>9020</v>
       </c>
       <c r="D28">
-        <v>9038</v>
+        <v>9014</v>
       </c>
       <c r="E28">
-        <v>9126</v>
+        <v>9178</v>
       </c>
       <c r="F28">
-        <v>9117</v>
+        <v>8954</v>
       </c>
       <c r="G28">
-        <v>8986</v>
+        <v>9200</v>
       </c>
       <c r="H28">
-        <v>8957</v>
+        <v>9112</v>
       </c>
       <c r="I28">
-        <v>9065</v>
+        <v>9138</v>
       </c>
       <c r="J28">
-        <v>9113</v>
+        <v>8916</v>
       </c>
       <c r="K28">
-        <v>9242</v>
+        <v>9160</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>9165</v>
+        <v>9122</v>
       </c>
       <c r="B29">
-        <v>9111</v>
+        <v>9090</v>
       </c>
       <c r="C29">
-        <v>9193</v>
+        <v>9128</v>
       </c>
       <c r="D29">
-        <v>9136</v>
+        <v>8949</v>
       </c>
       <c r="E29">
-        <v>9011</v>
+        <v>9060</v>
       </c>
       <c r="F29">
-        <v>9040</v>
+        <v>9218</v>
       </c>
       <c r="G29">
-        <v>9015</v>
+        <v>9134</v>
       </c>
       <c r="H29">
-        <v>8893</v>
+        <v>9229</v>
       </c>
       <c r="I29">
-        <v>9198</v>
+        <v>8901</v>
       </c>
       <c r="J29">
-        <v>9142</v>
+        <v>9073</v>
       </c>
       <c r="K29">
-        <v>9096</v>
+        <v>9093</v>
       </c>
       <c r="L29">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>9078</v>
+        <v>9030</v>
       </c>
       <c r="B30">
-        <v>9210</v>
+        <v>9075</v>
       </c>
       <c r="C30">
-        <v>8974</v>
+        <v>9191</v>
       </c>
       <c r="D30">
-        <v>9217</v>
+        <v>9211</v>
       </c>
       <c r="E30">
-        <v>9127</v>
+        <v>9112</v>
       </c>
       <c r="F30">
-        <v>9113</v>
+        <v>9005</v>
       </c>
       <c r="G30">
-        <v>9065</v>
+        <v>8958</v>
       </c>
       <c r="H30">
-        <v>9056</v>
+        <v>9172</v>
       </c>
       <c r="I30">
-        <v>9007</v>
+        <v>9142</v>
       </c>
       <c r="J30">
-        <v>8914</v>
+        <v>8979</v>
       </c>
       <c r="K30">
-        <v>9239</v>
+        <v>9121</v>
       </c>
       <c r="L30">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <f>AVERAGE(A1:A30)</f>
-        <v>9109.5</v>
+        <v>9115.4333333333325</v>
       </c>
       <c r="B31">
         <f>AVERAGE(B1:B30)</f>
-        <v>9094.7333333333336</v>
+        <v>9094.1333333333332</v>
       </c>
       <c r="C31">
         <f>AVERAGE(C1:C30)</f>
-        <v>9086.1666666666661</v>
+        <v>9091.1</v>
       </c>
       <c r="D31">
         <f>AVERAGE(D1:D30)</f>
-        <v>9079.0333333333328</v>
+        <v>9102.4</v>
       </c>
       <c r="E31">
         <f>AVERAGE(E1:E30)</f>
-        <v>9108.3666666666668</v>
+        <v>9070.1333333333332</v>
       </c>
       <c r="F31">
         <f>AVERAGE(F1:F30)</f>
-        <v>9069.1333333333332</v>
+        <v>9063.7666666666664</v>
       </c>
       <c r="G31">
         <f>AVERAGE(G1:G30)</f>
-        <v>9055.9</v>
+        <v>9102.9333333333325</v>
       </c>
       <c r="H31">
         <f>AVERAGE(H1:H30)</f>
-        <v>9122.0333333333328</v>
+        <v>9084.2333333333336</v>
       </c>
       <c r="I31">
         <f>AVERAGE(I1:I30)</f>
-        <v>9095.9333333333325</v>
+        <v>9102.7666666666664</v>
       </c>
       <c r="J31">
         <f>AVERAGE(J1:J30)</f>
-        <v>9099.8666666666668</v>
+        <v>9077.1666666666661</v>
       </c>
       <c r="K31">
         <f>AVERAGE(K1:K30)</f>
-        <v>9079.3333333333339</v>
+        <v>9092.5666666666675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>